<commit_message>
MAJ journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail/Journal_de_travaille_Antoine-Roulin.xlsx
+++ b/Documentation/Journal de travail/Journal_de_travaille_Antoine-Roulin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoi\Desktop\Cours\ICT-431\Journal de travail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BatailleNavale\BatailleNavale\Documentation\Journal de travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE0FC58-27FC-46BA-9E88-41614D4E66C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1274A853-9AB2-41EA-92E0-2B2B9F4137BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3270" yWindow="5655" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>DATE</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Correction des dernier bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création du sprint 4 + issues </t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +494,7 @@
         <v>0.47569444444444442</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D14" si="0">C2-B2</f>
+        <f t="shared" ref="D2:D15" si="0">C2-B2</f>
         <v>3.125E-2</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -730,11 +733,22 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="5"/>
+      <c r="A15" s="2">
+        <v>43906</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>